<commit_message>
MOdification message d'erreur quand excel n'est pas installé
</commit_message>
<xml_diff>
--- a/Scripts/01-config/02-modele-grille.xlsx
+++ b/Scripts/01-config/02-modele-grille.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\DataFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\Scripts\01-config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED682DA-6A44-48FB-9954-CD150E5746A8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654841E-E071-4B57-A4C6-9968AF49C96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51F219C5-3CFD-461A-AEFF-1CF380BD0F9C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51F219C5-3CFD-461A-AEFF-1CF380BD0F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="1" r:id="rId1"/>
@@ -1147,6 +1147,68 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" textRotation="90"/>
     </xf>
@@ -1163,68 +1225,6 @@
     <xf numFmtId="14" fontId="6" fillId="0" borderId="4" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="29" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="26" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="25" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="22" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="21" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="20" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="19" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="17" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1836,26 +1836,26 @@
     </row>
     <row r="5" spans="1:21" s="7" customFormat="1" ht="25.15" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C5" s="56"/>
-      <c r="D5" s="86" t="s">
+      <c r="D5" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="E5" s="87"/>
-      <c r="F5" s="87"/>
-      <c r="G5" s="88" t="s">
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="80" t="s">
         <v>32</v>
       </c>
-      <c r="H5" s="89"/>
-      <c r="I5" s="89"/>
-      <c r="J5" s="90" t="s">
+      <c r="H5" s="81"/>
+      <c r="I5" s="81"/>
+      <c r="J5" s="82" t="s">
         <v>31</v>
       </c>
-      <c r="K5" s="91"/>
-      <c r="L5" s="91"/>
-      <c r="M5" s="92" t="s">
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="84" t="s">
         <v>30</v>
       </c>
-      <c r="N5" s="93"/>
-      <c r="O5" s="93"/>
+      <c r="N5" s="85"/>
+      <c r="O5" s="85"/>
       <c r="P5" s="55" t="s">
         <v>29</v>
       </c>
@@ -1869,10 +1869,10 @@
       <c r="U5"/>
     </row>
     <row r="6" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="94" t="s">
+      <c r="A6" s="86" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="97" t="s">
+      <c r="B6" s="89" t="s">
         <v>25</v>
       </c>
       <c r="C6" s="52" t="s">
@@ -1920,8 +1920,8 @@
       <c r="U6"/>
     </row>
     <row r="7" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="95"/>
-      <c r="B7" s="98"/>
+      <c r="A7" s="87"/>
+      <c r="B7" s="90"/>
       <c r="C7" s="49" t="s">
         <v>22</v>
       </c>
@@ -1962,8 +1962,8 @@
       </c>
     </row>
     <row r="8" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="95"/>
-      <c r="B8" s="98"/>
+      <c r="A8" s="87"/>
+      <c r="B8" s="90"/>
       <c r="C8" s="49" t="s">
         <v>21</v>
       </c>
@@ -2004,8 +2004,8 @@
       </c>
     </row>
     <row r="9" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="95"/>
-      <c r="B9" s="99"/>
+      <c r="A9" s="87"/>
+      <c r="B9" s="91"/>
       <c r="C9" s="49" t="s">
         <v>20</v>
       </c>
@@ -2046,8 +2046,8 @@
       </c>
     </row>
     <row r="10" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="95"/>
-      <c r="B10" s="100" t="s">
+      <c r="A10" s="87"/>
+      <c r="B10" s="92" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="49" t="s">
@@ -2090,8 +2090,8 @@
       </c>
     </row>
     <row r="11" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="95"/>
-      <c r="B11" s="101"/>
+      <c r="A11" s="87"/>
+      <c r="B11" s="93"/>
       <c r="C11" s="49" t="s">
         <v>17</v>
       </c>
@@ -2133,8 +2133,8 @@
       <c r="R11" s="50"/>
     </row>
     <row r="12" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="95"/>
-      <c r="B12" s="102"/>
+      <c r="A12" s="87"/>
+      <c r="B12" s="94"/>
       <c r="C12" s="49" t="s">
         <v>16</v>
       </c>
@@ -2175,7 +2175,7 @@
       </c>
     </row>
     <row r="13" spans="1:21" s="18" customFormat="1" ht="75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="96"/>
+      <c r="A13" s="88"/>
       <c r="B13" s="34" t="s">
         <v>15</v>
       </c>
@@ -2225,81 +2225,81 @@
       <c r="L14" s="16"/>
       <c r="M14" s="16"/>
       <c r="N14" s="15"/>
-      <c r="O14" s="78" t="s">
+      <c r="O14" s="98" t="s">
         <v>7</v>
       </c>
       <c r="P14" s="13"/>
       <c r="Q14" s="14"/>
     </row>
     <row r="15" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="84" t="s">
+      <c r="A15" s="96" t="s">
         <v>6</v>
       </c>
-      <c r="B15" s="85"/>
-      <c r="C15" s="85"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="85"/>
-      <c r="F15" s="85"/>
-      <c r="G15" s="85"/>
-      <c r="H15" s="85"/>
-      <c r="J15" s="79" t="s">
+      <c r="B15" s="97"/>
+      <c r="C15" s="97"/>
+      <c r="D15" s="97"/>
+      <c r="E15" s="97"/>
+      <c r="F15" s="97"/>
+      <c r="G15" s="97"/>
+      <c r="H15" s="97"/>
+      <c r="J15" s="99" t="s">
         <v>5</v>
       </c>
-      <c r="K15" s="79"/>
-      <c r="L15" s="82"/>
-      <c r="M15" s="82"/>
-      <c r="N15" s="82"/>
-      <c r="O15" s="78"/>
+      <c r="K15" s="99"/>
+      <c r="L15" s="102"/>
+      <c r="M15" s="102"/>
+      <c r="N15" s="102"/>
+      <c r="O15" s="98"/>
       <c r="P15" s="13"/>
     </row>
     <row r="16" spans="1:21" s="7" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="84" t="s">
+      <c r="A16" s="96" t="s">
         <v>4</v>
       </c>
-      <c r="B16" s="85"/>
-      <c r="C16" s="85"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="85"/>
-      <c r="F16" s="85"/>
-      <c r="G16" s="85"/>
-      <c r="H16" s="85"/>
-      <c r="J16" s="80" t="s">
+      <c r="B16" s="97"/>
+      <c r="C16" s="97"/>
+      <c r="D16" s="97"/>
+      <c r="E16" s="97"/>
+      <c r="F16" s="97"/>
+      <c r="G16" s="97"/>
+      <c r="H16" s="97"/>
+      <c r="J16" s="100" t="s">
         <v>3</v>
       </c>
-      <c r="K16" s="80"/>
-      <c r="L16" s="81"/>
-      <c r="M16" s="81"/>
-      <c r="N16" s="81"/>
+      <c r="K16" s="100"/>
+      <c r="L16" s="101"/>
+      <c r="M16" s="101"/>
+      <c r="N16" s="101"/>
       <c r="O16" s="12"/>
       <c r="P16" s="12"/>
       <c r="Q16" s="11"/>
     </row>
     <row r="17" spans="1:17" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="84"/>
-      <c r="B17" s="85"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="85"/>
-      <c r="F17" s="85"/>
-      <c r="G17" s="85"/>
-      <c r="H17" s="85"/>
+      <c r="A17" s="96"/>
+      <c r="B17" s="97"/>
+      <c r="C17" s="97"/>
+      <c r="D17" s="97"/>
+      <c r="E17" s="97"/>
+      <c r="F17" s="97"/>
+      <c r="G17" s="97"/>
+      <c r="H17" s="97"/>
       <c r="K17" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="L17" s="81"/>
-      <c r="M17" s="81"/>
-      <c r="N17" s="81"/>
+      <c r="L17" s="101"/>
+      <c r="M17" s="101"/>
+      <c r="N17" s="101"/>
       <c r="Q17" s="9"/>
     </row>
     <row r="18" spans="1:17" s="7" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="84"/>
-      <c r="B18" s="85"/>
-      <c r="C18" s="85"/>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
+      <c r="A18" s="96"/>
+      <c r="B18" s="97"/>
+      <c r="C18" s="97"/>
+      <c r="D18" s="97"/>
+      <c r="E18" s="97"/>
+      <c r="F18" s="97"/>
+      <c r="G18" s="97"/>
+      <c r="H18" s="97"/>
       <c r="N18" s="7" t="s">
         <v>1</v>
       </c>
@@ -2309,9 +2309,9 @@
       </c>
     </row>
     <row r="19" spans="1:17" ht="20.25" hidden="1" x14ac:dyDescent="0.3">
-      <c r="K19" s="83"/>
-      <c r="L19" s="83"/>
-      <c r="M19" s="83"/>
+      <c r="K19" s="95"/>
+      <c r="L19" s="95"/>
+      <c r="M19" s="95"/>
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.2"/>
     <row r="22" spans="1:17" ht="15" hidden="1" x14ac:dyDescent="0.25">
@@ -2380,6 +2380,17 @@
     <protectedRange sqref="D6:Q13 L15 L16 L17 A15:H18" name="Cellules modifiables"/>
   </protectedRanges>
   <mergeCells count="18">
+    <mergeCell ref="O14:O15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="J16:K16"/>
+    <mergeCell ref="L17:N17"/>
+    <mergeCell ref="L15:N15"/>
+    <mergeCell ref="L16:N16"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="A15:H15"/>
+    <mergeCell ref="A16:H16"/>
+    <mergeCell ref="A17:H17"/>
+    <mergeCell ref="A18:H18"/>
     <mergeCell ref="D5:F5"/>
     <mergeCell ref="G5:I5"/>
     <mergeCell ref="J5:L5"/>
@@ -2387,17 +2398,6 @@
     <mergeCell ref="A6:A13"/>
     <mergeCell ref="B6:B9"/>
     <mergeCell ref="B10:B12"/>
-    <mergeCell ref="K19:M19"/>
-    <mergeCell ref="A15:H15"/>
-    <mergeCell ref="A16:H16"/>
-    <mergeCell ref="A17:H17"/>
-    <mergeCell ref="A18:H18"/>
-    <mergeCell ref="O14:O15"/>
-    <mergeCell ref="J15:K15"/>
-    <mergeCell ref="J16:K16"/>
-    <mergeCell ref="L17:N17"/>
-    <mergeCell ref="L15:N15"/>
-    <mergeCell ref="L16:N16"/>
   </mergeCells>
   <conditionalFormatting sqref="Q18">
     <cfRule type="cellIs" dxfId="11" priority="1" operator="equal">

</xml_diff>

<commit_message>
Mise à jour des modèles
</commit_message>
<xml_diff>
--- a/Scripts/01-config/02-modele-grille.xlsx
+++ b/Scripts/01-config/02-modele-grille.xlsx
@@ -2,21 +2,22 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\09-P_Appro\PS-Eval\Scripts\01-config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6654841E-E071-4B57-A4C6-9968AF49C96E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80E97EC5-F577-4FF5-806E-CF84373A8AAA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51F219C5-3CFD-461A-AEFF-1CF380BD0F9C}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{51F219C5-3CFD-461A-AEFF-1CF380BD0F9C}"/>
   </bookViews>
   <sheets>
     <sheet name="MASTER" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="CLASSE">MASTER!$E$3</definedName>
+    <definedName name="CLASSROOM">MASTER!$E$3</definedName>
     <definedName name="cst_A">MASTER!$S$3</definedName>
     <definedName name="cst_ERR">MASTER!$S$6</definedName>
     <definedName name="cst_ignore">MASTER!$T$1</definedName>
@@ -26,6 +27,7 @@
     <definedName name="cst_NA">MASTER!$S$5</definedName>
     <definedName name="cst_PA">MASTER!$S$4</definedName>
     <definedName name="DATES">MASTER!$J$4</definedName>
+    <definedName name="DATESMERGED">MASTER!$J$4</definedName>
     <definedName name="FINALNOTE">MASTER!$Q$18</definedName>
     <definedName name="NAME">MASTER!$E$2</definedName>
     <definedName name="NBWEEKS">MASTER!$J$3</definedName>
@@ -239,22 +241,22 @@
     <t xml:space="preserve">ÉVALUATION DES COMPÉTENCES EN PRATIQUE POUR LA FORMATION </t>
   </si>
   <si>
-    <t>[NAME]</t>
-  </si>
-  <si>
-    <t>[CLASSE]</t>
-  </si>
-  <si>
-    <t>[TEACHER]</t>
-  </si>
-  <si>
-    <t>[PROJECTNAME]</t>
-  </si>
-  <si>
-    <t>[NBWEEKS]</t>
-  </si>
-  <si>
-    <t>[DATES]</t>
+    <t>NAME</t>
+  </si>
+  <si>
+    <t>TEACHER</t>
+  </si>
+  <si>
+    <t>PROJECTNAME</t>
+  </si>
+  <si>
+    <t>NBWEEKS</t>
+  </si>
+  <si>
+    <t>DATESMERGED</t>
+  </si>
+  <si>
+    <t>CLASSROOM</t>
   </si>
 </sst>
 </file>
@@ -1698,10 +1700,10 @@
   <sheetPr codeName="Feuil3">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U33"/>
+  <dimension ref="A1:U36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.85546875" defaultRowHeight="12.75" zeroHeight="1" x14ac:dyDescent="0.2"/>
@@ -1755,7 +1757,7 @@
         <v>41</v>
       </c>
       <c r="J2" s="72" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K2" s="71"/>
       <c r="L2" s="71"/>
@@ -1778,7 +1780,7 @@
         <v>39</v>
       </c>
       <c r="E3" s="69" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F3" s="67"/>
       <c r="G3" s="67"/>
@@ -1787,7 +1789,7 @@
         <v>38</v>
       </c>
       <c r="J3" s="69" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="K3" s="68"/>
       <c r="L3" s="67"/>
@@ -1810,7 +1812,7 @@
         <v>36</v>
       </c>
       <c r="E4" s="63" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F4" s="58"/>
       <c r="G4" s="58"/>
@@ -1819,7 +1821,7 @@
         <v>35</v>
       </c>
       <c r="J4" s="60" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K4" s="59"/>
       <c r="L4" s="58"/>
@@ -2374,10 +2376,13 @@
         <v>6</v>
       </c>
     </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sheetProtection sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1"/>
   <protectedRanges>
-    <protectedRange sqref="D6:Q13 L15 L16 L17 A15:H18" name="Cellules modifiables"/>
+    <protectedRange sqref="L15:L17 A15:H18 D6:Q13" name="Cellules modifiables"/>
   </protectedRanges>
   <mergeCells count="18">
     <mergeCell ref="O14:O15"/>

</xml_diff>